<commit_message>
chore: update test excel with a nan
</commit_message>
<xml_diff>
--- a/tests/test_files/test.xlsx
+++ b/tests/test_files/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m1a1/Developer/markitdown/tests/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA45145-359B-6341-85DE-824EBC0A5BC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186CC3EF-31FC-844A-BFFA-52F1C80738E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1720" yWindow="1840" windowWidth="31100" windowHeight="19420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -395,9 +395,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="158" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="158" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -618,9 +616,6 @@
       </c>
       <c r="E13">
         <v>67</v>
-      </c>
-      <c r="F13">
-        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
chore: consider header for column-wise drop
</commit_message>
<xml_diff>
--- a/tests/test_files/test.xlsx
+++ b/tests/test_files/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m1a1/Developer/markitdown/tests/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186CC3EF-31FC-844A-BFFA-52F1C80738E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578E885C-5ED3-3E4D-9FCE-6E1F2AD347E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1720" yWindow="1840" windowWidth="31100" windowHeight="19420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -393,9 +393,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="158" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="158" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -452,252 +454,241 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>60</v>
-      </c>
-      <c r="C4">
-        <v>84</v>
-      </c>
-      <c r="D4">
-        <v>19</v>
-      </c>
-      <c r="E4">
-        <v>19</v>
-      </c>
-      <c r="F4">
-        <v>53</v>
+      <c r="A4" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="C5">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="D5">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E5">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F5">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>87</v>
+        <v>7</v>
       </c>
       <c r="C6">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="D6">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="E6">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="F6">
-        <v>312</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>89</v>
       </c>
       <c r="D7">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E7">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="F7">
-        <v>23</v>
+        <v>312</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>70</v>
+        <v>23</v>
       </c>
       <c r="C8">
-        <v>84</v>
+        <v>4</v>
       </c>
       <c r="D8">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="E8">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="F8">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="C9">
-        <v>37</v>
+        <v>84</v>
       </c>
       <c r="D9">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="E9">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="F9">
-        <v>321</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="C10">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="D10">
-        <v>88</v>
+        <v>43</v>
       </c>
       <c r="E10">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="F10">
-        <v>431</v>
+        <v>321</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="C11">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="D11">
-        <v>20</v>
+        <v>88</v>
       </c>
       <c r="E11">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="F11">
-        <v>647</v>
+        <v>431</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>62</v>
+      </c>
+      <c r="D12">
+        <v>20</v>
+      </c>
+      <c r="E12">
         <v>67</v>
       </c>
-      <c r="C12">
-        <v>18</v>
-      </c>
-      <c r="D12">
-        <v>15</v>
-      </c>
-      <c r="E12">
-        <v>48</v>
-      </c>
       <c r="F12">
-        <v>878</v>
+        <v>647</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="C13">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D13">
         <v>15</v>
       </c>
       <c r="E13">
-        <v>67</v>
+        <v>48</v>
+      </c>
+      <c r="F13">
+        <v>878</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>58</v>
-      </c>
-      <c r="C14" t="s">
-        <v>9</v>
+        <v>42</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
       </c>
       <c r="D14">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E14">
-        <v>9</v>
-      </c>
-      <c r="F14">
-        <v>346</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>49</v>
-      </c>
-      <c r="C15">
-        <v>93</v>
+        <v>58</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
       </c>
       <c r="D15">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="E15">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="F15">
-        <v>317</v>
+        <v>346</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>82</v>
+        <v>49</v>
       </c>
       <c r="C16">
-        <v>28</v>
+        <v>93</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E16">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F16">
-        <v>341</v>
+        <v>317</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="C17">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="D17">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="E17">
-        <v>82</v>
+        <v>39</v>
       </c>
       <c r="F17">
-        <v>135</v>
+        <v>341</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="C18">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="D18">
-        <v>98</v>
+        <v>18</v>
       </c>
       <c r="E18">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F18">
         <v>135</v>
@@ -705,103 +696,120 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="C19">
         <v>46</v>
       </c>
       <c r="D19">
-        <v>47</v>
+        <v>98</v>
       </c>
       <c r="E19">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="F19">
-        <v>3634</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C20">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="D20">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="E20">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="F20">
-        <v>357</v>
+        <v>3634</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>95</v>
+        <v>40</v>
       </c>
       <c r="C21">
         <v>65</v>
       </c>
       <c r="D21">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E21">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="F21">
-        <v>34</v>
+        <v>357</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>68</v>
+        <v>95</v>
       </c>
       <c r="C22">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D22">
+        <v>29</v>
+      </c>
+      <c r="E22">
+        <v>62</v>
+      </c>
+      <c r="F22">
         <v>34</v>
-      </c>
-      <c r="E22">
-        <v>54</v>
-      </c>
-      <c r="F22">
-        <v>901</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>96</v>
+        <v>68</v>
       </c>
       <c r="C23">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D23">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="E23">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="F23">
-        <v>299</v>
+        <v>901</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
+        <v>96</v>
+      </c>
+      <c r="C24">
+        <v>66</v>
+      </c>
+      <c r="D24">
+        <v>63</v>
+      </c>
+      <c r="E24">
+        <v>14</v>
+      </c>
+      <c r="F24">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25">
         <v>87</v>
       </c>
-      <c r="C24">
+      <c r="C25">
         <v>93</v>
       </c>
-      <c r="D24">
+      <c r="D25">
         <v>95</v>
       </c>
-      <c r="E24">
+      <c r="E25">
         <v>80</v>
       </c>
-      <c r="F24">
+      <c r="F25">
         <v>19</v>
       </c>
     </row>

</xml_diff>